<commit_message>
Split score and evaluation, add loading status
</commit_message>
<xml_diff>
--- a/templates/ket_qua_kiem_tra.xlsx
+++ b/templates/ket_qua_kiem_tra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duy Long\Desktop\NCKH\Quản lý sinh viên\quanlysinhvien\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703DBFF0-482E-4285-AE73-1442A66C0597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0D9ACE5-B100-4313-B0F4-7D461A469978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Mã học sinh</t>
   </si>
@@ -61,15 +61,6 @@
   </si>
   <si>
     <t>Điểm tổng kết</t>
-  </si>
-  <si>
-    <t>Hạnh kiểm</t>
-  </si>
-  <si>
-    <t>Học lực</t>
-  </si>
-  <si>
-    <t>Xếp loại</t>
   </si>
 </sst>
 </file>
@@ -408,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -424,13 +415,10 @@
     <col min="9" max="10" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="2"/>
+    <col min="13" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,35 +455,8 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sai giá trị" error="Tốt, Khá, Yếu" sqref="M2:M1048576" xr:uid="{D2265C54-68CC-4666-B901-D03416005934}">
-      <formula1>"Tốt, Khá, Yếu"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sai giá trị" error="Giỏi, Khá, Trung bình" sqref="N2:N1048576 N2:N1048576" xr:uid="{7BD16EFA-0AC6-4E1D-A6CB-C3B943999D1D}">
-      <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-        <mc:Choice Requires="x12ac">
-          <x12ac:list>"Giỏi, Khá, Trung bình"</x12ac:list>
-        </mc:Choice>
-        <mc:Fallback>
-          <formula1>"Giỏi, Khá, Trung bình"</formula1>
-        </mc:Fallback>
-      </mc:AlternateContent>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Sai giá trị" error="Giỏi; Khá; Trung bình; Yếu" sqref="O2:O1048576" xr:uid="{B3D2D12D-3F48-4C7E-AF9C-801B9043067A}">
-      <formula1>"Giỏi, Khá, Trung bình, Yếu"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>